<commit_message>
Aufgabe a,b,c und 1.1
</commit_message>
<xml_diff>
--- a/Dossier.xlsx
+++ b/Dossier.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\49152\Desktop\Fh Aachen\3. Semester\DBWT\M3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fhaachen-my.sharepoint.com/personal/nh1236s_ad_fh-aachen_de/Documents/Semester 3/DBWT/Praktika/DBWT_M6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B751F3D7-05B9-49FA-937C-00207C51B9F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="110" documentId="13_ncr:1_{B751F3D7-05B9-49FA-937C-00207C51B9F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C7C01DB-1227-4283-B652-7B520EA19DA0}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7110" yWindow="2745" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Aufgabe_3" sheetId="2" r:id="rId2"/>
-    <sheet name="Aufgabe6" sheetId="3" r:id="rId3"/>
+    <sheet name="M6" sheetId="6" r:id="rId1"/>
+    <sheet name="M5" sheetId="3" r:id="rId2"/>
+    <sheet name="M4" sheetId="2" r:id="rId3"/>
+    <sheet name="M3" sheetId="1" r:id="rId4"/>
+    <sheet name="M2" sheetId="4" r:id="rId5"/>
+    <sheet name="M1" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,8 +32,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
   <si>
     <t>Aufgabe</t>
   </si>
@@ -86,6 +87,81 @@
   </si>
   <si>
     <t>Aufgabestellung ist nicht präsiz</t>
+  </si>
+  <si>
+    <t>Aufgabe 3</t>
+  </si>
+  <si>
+    <t>Aufgabe 6</t>
+  </si>
+  <si>
+    <t>seltsame Fehler</t>
+  </si>
+  <si>
+    <t>css Probleme</t>
+  </si>
+  <si>
+    <t>In Wunschgericht.php wäre SQL injektion möglich gewesen, jedoch kein XSS Injektion. Behoben durch mysqli_real_escape_string()</t>
+  </si>
+  <si>
+    <t>4) sehr komplex, konnte nichts finden über google</t>
+  </si>
+  <si>
+    <t>war einfacher als erwartet</t>
+  </si>
+  <si>
+    <t>a)</t>
+  </si>
+  <si>
+    <t>Unscheinbarer Fehler durch falschen Pfad</t>
+  </si>
+  <si>
+    <t>b)</t>
+  </si>
+  <si>
+    <t>ging nicht mit @splitforeach</t>
+  </si>
+  <si>
+    <t>c)</t>
+  </si>
+  <si>
+    <t>gericht.php war nicht eingebunden</t>
+  </si>
+  <si>
+    <t>d)</t>
+  </si>
+  <si>
+    <t>probleme mit css</t>
+  </si>
+  <si>
+    <t>Schwierigkeiten bei Aufgabe 4, mit Controller</t>
+  </si>
+  <si>
+    <t>Einlesen der Namen klappte nicht sofort</t>
+  </si>
+  <si>
+    <t>Einarbeiten in Monolog hat länger gedauert</t>
+  </si>
+  <si>
+    <t>Arbeitsaufwand etwas unterschätzt</t>
+  </si>
+  <si>
+    <t>Reinarbeiten in SQL-View dauerte etwas</t>
+  </si>
+  <si>
+    <t>Prozedur komplizierter als gedacht</t>
+  </si>
+  <si>
+    <t>einfacher als gedacht</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
   </si>
 </sst>
 </file>
@@ -137,7 +213,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -145,21 +221,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -447,22 +535,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F23473-93C6-4608-A05A-AD57ACA416C3}">
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -480,19 +565,622 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
       <c r="C2">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40E16A22-C1D6-4964-9FAE-9D54F9F0612D}">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>120</v>
+      </c>
+      <c r="D2">
+        <v>240</v>
+      </c>
+      <c r="E2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>15</v>
+      </c>
+      <c r="D4">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>30</v>
+      </c>
+      <c r="D8">
+        <v>60</v>
+      </c>
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <v>30</v>
+      </c>
+      <c r="E9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>30</v>
+      </c>
+      <c r="D10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>30</v>
+      </c>
+      <c r="D11">
+        <v>60</v>
+      </c>
+      <c r="E11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>30</v>
+      </c>
+      <c r="D12">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>30</v>
+      </c>
+      <c r="D13">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>30</v>
+      </c>
+      <c r="D15">
+        <v>50</v>
+      </c>
+      <c r="E15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{465C2EDA-7F18-4583-BE3C-89F9FAE038A2}">
+  <dimension ref="A1:F19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>15</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>60</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>40</v>
+      </c>
+      <c r="D10">
+        <v>60</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>30</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>30</v>
+      </c>
+      <c r="D12">
+        <v>15</v>
+      </c>
+      <c r="E12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13">
+        <v>15</v>
+      </c>
+      <c r="D13">
+        <v>40</v>
+      </c>
+      <c r="E13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14">
+        <v>20</v>
+      </c>
+      <c r="D14">
+        <v>60</v>
+      </c>
+      <c r="E14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15">
+        <v>15</v>
+      </c>
+      <c r="D15">
+        <v>20</v>
+      </c>
+      <c r="E15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16">
+        <v>30</v>
+      </c>
+      <c r="D16">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>120</v>
+      </c>
+      <c r="D17">
+        <v>210</v>
+      </c>
+      <c r="E17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5" t="str">
+        <f>(SUM(C2:C17))/60&amp;" Stunden"</f>
+        <v>6,1 Stunden</v>
+      </c>
+      <c r="D18" s="5" t="str">
+        <f>(SUM(D2:D17))/60&amp;" Stunden"</f>
+        <v>9,35 Stunden</v>
+      </c>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
         <v>3</v>
       </c>
       <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K2" s="3">
+        <v>1</v>
+      </c>
+      <c r="L2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -506,8 +1194,14 @@
         <v>5</v>
       </c>
       <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K3" s="3">
+        <v>2</v>
+      </c>
+      <c r="L3" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -520,8 +1214,14 @@
       <c r="E4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K4" s="3">
+        <v>3</v>
+      </c>
+      <c r="L4" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -534,8 +1234,14 @@
       <c r="E5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K5" s="3">
+        <v>4</v>
+      </c>
+      <c r="L5" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -546,8 +1252,14 @@
         <v>2</v>
       </c>
       <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K6" s="3">
+        <v>5</v>
+      </c>
+      <c r="L6" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -558,8 +1270,11 @@
         <v>30</v>
       </c>
       <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K7" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -572,8 +1287,11 @@
       <c r="E8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K8" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -587,8 +1305,11 @@
         <v>20</v>
       </c>
       <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K9" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>2</v>
       </c>
@@ -601,8 +1322,11 @@
       <c r="E10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K10" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>3</v>
       </c>
@@ -613,8 +1337,11 @@
         <v>10</v>
       </c>
       <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K11" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6</v>
       </c>
@@ -627,8 +1354,11 @@
       <c r="E12" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K12" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>7</v>
       </c>
@@ -642,7 +1372,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>8</v>
       </c>
@@ -654,7 +1384,7 @@
       </c>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>9</v>
       </c>
@@ -665,7 +1395,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>11</v>
       </c>
@@ -679,7 +1409,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C18">
         <f>SUM(C2:C16)</f>
         <v>296</v>
@@ -695,138 +1425,51 @@
       <formula>"C=D"</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="K3" r:id="rId1" display="Screenshots A3/2022-11-08 (1).png" xr:uid="{D13DB1AC-2E43-4845-9D55-54DF80CDEAAC}"/>
+    <hyperlink ref="K4" r:id="rId2" display="Screenshots A3/2022-11-08 (2).png" xr:uid="{F545C0DB-8F39-43D4-87CB-2049530D82C5}"/>
+    <hyperlink ref="K5" r:id="rId3" display="Screenshots A3/2022-11-08 (3).png" xr:uid="{789308EE-AB93-4941-8119-E07F3E6D0975}"/>
+    <hyperlink ref="K6" r:id="rId4" display="Screenshots A3/2022-11-08 (4).png" xr:uid="{220F2DEA-52F4-4DA2-96E4-3ACB6F60FD26}"/>
+    <hyperlink ref="K7" r:id="rId5" display="Screenshots A3/2022-11-08 (5).png" xr:uid="{421906C1-C874-4F82-919C-F2D732A7578A}"/>
+    <hyperlink ref="K8" r:id="rId6" display="Screenshots A3/2022-11-08 (6).png" xr:uid="{B8911758-9768-4B4A-94EC-DFD151121E8F}"/>
+    <hyperlink ref="K9" r:id="rId7" display="Screenshots A3/2022-11-08 (7).png" xr:uid="{19B92AB8-5B15-42B3-97A5-0F178BC1B792}"/>
+    <hyperlink ref="K10" r:id="rId8" display="Screenshots A3/2022-11-08 (8).png" xr:uid="{1A7B4269-0EE4-4B25-80DA-11E07CA34776}"/>
+    <hyperlink ref="K11" r:id="rId9" display="Screenshots A3/2022-11-08 (9).png" xr:uid="{83FD8BA7-4783-4917-A31D-6FD5DF46BA28}"/>
+    <hyperlink ref="K12" r:id="rId10" display="Screenshots A3/2022-11-08 (10).png" xr:uid="{D1CB6D4A-FC17-45C5-8517-5EC6C9C79C46}"/>
+    <hyperlink ref="K2" r:id="rId11" display="Screenshots A3/2022-11-08.png" xr:uid="{7C60811A-895E-4700-B991-C1566D2D29A3}"/>
+    <hyperlink ref="L2" r:id="rId12" display="1" xr:uid="{82C15182-40CC-416D-BB8E-B392868374C4}"/>
+    <hyperlink ref="L3" r:id="rId13" display="Scrrenshots A6/2022-11-10 (1).png" xr:uid="{19B599FE-F8B5-47B5-B32F-910809E1168A}"/>
+    <hyperlink ref="L4" r:id="rId14" display="Scrrenshots A6/2022-11-10 (2).png" xr:uid="{49482DE1-DC58-4CFC-B143-726A8BF4BB5B}"/>
+    <hyperlink ref="L5" r:id="rId15" display="Scrrenshots A6/2022-11-10 (3).png" xr:uid="{232841DD-8F45-4045-84FD-4F53E64CF79D}"/>
+    <hyperlink ref="L6" r:id="rId16" display="Scrrenshots A6/5.PNG" xr:uid="{CBB18311-2CB8-458D-AA55-799EC783DD25}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId17"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{465C2EDA-7F18-4583-BE3C-89F9FAE038A2}">
-  <dimension ref="A1:B11"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92058FDE-B750-446D-A360-4A10127FE0E9}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="3">
-        <v>1</v>
-      </c>
-      <c r="B1" s="3"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="3">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="3">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="Screenshots A3/2022-11-08 (1).png" xr:uid="{D13DB1AC-2E43-4845-9D55-54DF80CDEAAC}"/>
-    <hyperlink ref="A3" r:id="rId2" display="Screenshots A3/2022-11-08 (2).png" xr:uid="{F545C0DB-8F39-43D4-87CB-2049530D82C5}"/>
-    <hyperlink ref="A4" r:id="rId3" display="Screenshots A3/2022-11-08 (3).png" xr:uid="{789308EE-AB93-4941-8119-E07F3E6D0975}"/>
-    <hyperlink ref="A5" r:id="rId4" display="Screenshots A3/2022-11-08 (4).png" xr:uid="{220F2DEA-52F4-4DA2-96E4-3ACB6F60FD26}"/>
-    <hyperlink ref="A6" r:id="rId5" display="Screenshots A3/2022-11-08 (5).png" xr:uid="{421906C1-C874-4F82-919C-F2D732A7578A}"/>
-    <hyperlink ref="A7" r:id="rId6" display="Screenshots A3/2022-11-08 (6).png" xr:uid="{B8911758-9768-4B4A-94EC-DFD151121E8F}"/>
-    <hyperlink ref="A8" r:id="rId7" display="Screenshots A3/2022-11-08 (7).png" xr:uid="{19B92AB8-5B15-42B3-97A5-0F178BC1B792}"/>
-    <hyperlink ref="A9" r:id="rId8" display="Screenshots A3/2022-11-08 (8).png" xr:uid="{1A7B4269-0EE4-4B25-80DA-11E07CA34776}"/>
-    <hyperlink ref="A10" r:id="rId9" display="Screenshots A3/2022-11-08 (9).png" xr:uid="{83FD8BA7-4783-4917-A31D-6FD5DF46BA28}"/>
-    <hyperlink ref="A11" r:id="rId10" display="Screenshots A3/2022-11-08 (10).png" xr:uid="{D1CB6D4A-FC17-45C5-8517-5EC6C9C79C46}"/>
-    <hyperlink ref="A1" r:id="rId11" display="Screenshots A3/2022-11-08.png" xr:uid="{7C60811A-895E-4700-B991-C1566D2D29A3}"/>
-  </hyperlinks>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40E16A22-C1D6-4964-9FAE-9D54F9F0612D}">
-  <dimension ref="A1:A5"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B068C48-9658-4E2B-B234-7111A55F406D}">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" s="3">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="1" xr:uid="{82C15182-40CC-416D-BB8E-B392868374C4}"/>
-    <hyperlink ref="A2" r:id="rId2" display="Scrrenshots A6/2022-11-10 (1).png" xr:uid="{19B599FE-F8B5-47B5-B32F-910809E1168A}"/>
-    <hyperlink ref="A3" r:id="rId3" display="Scrrenshots A6/2022-11-10 (2).png" xr:uid="{49482DE1-DC58-4CFC-B143-726A8BF4BB5B}"/>
-    <hyperlink ref="A4" r:id="rId4" display="Scrrenshots A6/2022-11-10 (3).png" xr:uid="{232841DD-8F45-4045-84FD-4F53E64CF79D}"/>
-    <hyperlink ref="A5" r:id="rId5" display="Scrrenshots A6/5.PNG" xr:uid="{CBB18311-2CB8-458D-AA55-799EC783DD25}"/>
-  </hyperlinks>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Aufgabe 1.7 Viele sachen aus M5 hinzugefügt, die leider fehlten. Kaotisches Projekt..
</commit_message>
<xml_diff>
--- a/Dossier.xlsx
+++ b/Dossier.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fhaachen-my.sharepoint.com/personal/nh1236s_ad_fh-aachen_de/Documents/Semester 3/DBWT/Praktika/DBWT_M6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="125" documentId="13_ncr:1_{B751F3D7-05B9-49FA-937C-00207C51B9F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7AB178C7-A3FB-4388-A052-614CB907EEC2}"/>
+  <xr:revisionPtr revIDLastSave="134" documentId="13_ncr:1_{B751F3D7-05B9-49FA-937C-00207C51B9F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A34F6F9-21C7-4610-B980-7AE4844858F0}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="7110" yWindow="2745" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7110" yWindow="2745" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="M6" sheetId="6" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
   <si>
     <t>Aufgabe</t>
   </si>
@@ -168,6 +168,12 @@
   </si>
   <si>
     <t>Probleme beim auflösen des Dateipfades zum Bild</t>
+  </si>
+  <si>
+    <t>css probleme</t>
+  </si>
+  <si>
+    <t>Flow war da</t>
   </si>
 </sst>
 </file>
@@ -542,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F23473-93C6-4608-A05A-AD57ACA416C3}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,6 +678,34 @@
       </c>
       <c r="E9" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>20</v>
+      </c>
+      <c r="D10">
+        <v>30</v>
+      </c>
+      <c r="E10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>30</v>
+      </c>
+      <c r="D11">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>